<commit_message>
hidden files extracted, unhidden and copied here
might have to change the names later though
</commit_message>
<xml_diff>
--- a/resources/T4.1-Tools-for-Ancillary-Services-Procurement-in-day-ahead-operation-planning-of-Distrib.-Networks-main/output_data/March2023_LoadDataFromAttestCloud/EditedInputFiles/OutLog.xlsx
+++ b/resources/T4.1-Tools-for-Ancillary-Services-Procurement-in-day-ahead-operation-planning-of-Distrib.-Networks-main/output_data/March2023_LoadDataFromAttestCloud/EditedInputFiles/OutLog.xlsx
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="30">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="32">
   <si>
     <t>#</t>
   </si>
@@ -115,6 +115,12 @@
   </si>
   <si>
     <t>2024-02-16T04:02:53.451</t>
+  </si>
+  <si>
+    <t>2024-02-16T04:07:11.353</t>
+  </si>
+  <si>
+    <t>2024-02-16T04:08:15.245</t>
   </si>
 </sst>
 </file>
@@ -466,7 +472,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CAF0E20E-E4D8-9B45-9C94-E89B574F109C}">
-  <dimension ref="A1:I6"/>
+  <dimension ref="A1:I8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -646,6 +652,64 @@
         <v>0</v>
       </c>
     </row>
+    <row r="7" spans="1:9">
+      <c r="A7">
+        <v>33</v>
+      </c>
+      <c r="B7" t="s">
+        <v>26</v>
+      </c>
+      <c r="C7" t="s">
+        <v>27</v>
+      </c>
+      <c r="D7" t="s">
+        <v>28</v>
+      </c>
+      <c r="E7" t="s">
+        <v>30</v>
+      </c>
+      <c r="F7" t="s">
+        <v>13</v>
+      </c>
+      <c r="G7" t="b">
+        <v>0</v>
+      </c>
+      <c r="H7" t="b">
+        <v>0</v>
+      </c>
+      <c r="I7" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9">
+      <c r="A8">
+        <v>33</v>
+      </c>
+      <c r="B8" t="s">
+        <v>26</v>
+      </c>
+      <c r="C8" t="s">
+        <v>27</v>
+      </c>
+      <c r="D8" t="s">
+        <v>28</v>
+      </c>
+      <c r="E8" t="s">
+        <v>31</v>
+      </c>
+      <c r="F8" t="s">
+        <v>13</v>
+      </c>
+      <c r="G8" t="b">
+        <v>0</v>
+      </c>
+      <c r="H8" t="b">
+        <v>0</v>
+      </c>
+      <c r="I8" t="b">
+        <v>0</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>